<commit_message>
Added "PersonIndexIdentification" element to the IEPD.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Behavioral_Health_Evalutation_Reporting/artifacts/service_model/information_model/IEPD/documentation/BehaviorHealthReportMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Behavioral_Health_Evalutation_Reporting/artifacts/service_model/information_model/IEPD/documentation/BehaviorHealthReportMapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="-28120" yWindow="6400" windowWidth="28800" windowHeight="16060" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
   <si>
     <t>Race</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>Name of provider that completed the assessment</t>
+  </si>
+  <si>
+    <t>Person Index ID</t>
+  </si>
+  <si>
+    <t>A unique index identifier for a person</t>
   </si>
 </sst>
 </file>
@@ -2252,11 +2258,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFA350"/>
+  <dimension ref="A1:XFA351"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -35446,22 +35452,20 @@
       <c r="K20" s="24"/>
       <c r="L20" s="20"/>
     </row>
-    <row r="21" spans="1:12" s="19" customFormat="1">
-      <c r="A21" s="12" t="s">
-        <v>26</v>
+    <row r="21" spans="1:12" s="19" customFormat="1" ht="30">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7" t="s">
+        <v>78</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>60</v>
+      <c r="C21" s="7" t="s">
+        <v>79</v>
       </c>
-      <c r="C21" s="7"/>
       <c r="D21" s="22"/>
       <c r="E21" s="23"/>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
       <c r="H21" s="24"/>
-      <c r="I21" s="22" t="s">
-        <v>47</v>
-      </c>
+      <c r="I21" s="24"/>
       <c r="J21" s="24"/>
       <c r="K21" s="24"/>
       <c r="L21" s="20"/>
@@ -35471,7 +35475,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="22"/>
@@ -35491,12 +35495,10 @@
         <v>26</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="23"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="23"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
@@ -35513,193 +35515,190 @@
         <v>26</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="25" t="s">
+      <c r="I24" s="22" t="s">
         <v>47</v>
       </c>
       <c r="J24" s="24"/>
       <c r="K24" s="24"/>
       <c r="L24" s="20"/>
     </row>
-    <row r="25" spans="1:12" ht="51.75" customHeight="1">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6" t="s">
+    <row r="25" spans="1:12" s="19" customFormat="1">
+      <c r="A25" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="20"/>
+    </row>
+    <row r="26" spans="1:12" ht="51.75" customHeight="1">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="5" t="s">
+      <c r="D26" s="11"/>
+      <c r="E26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5" t="s">
+      <c r="F26" s="5"/>
+      <c r="G26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="18" t="s">
+      <c r="I26" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="35" t="s">
+    <row r="27" spans="1:12">
+      <c r="A27" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
     </row>
-    <row r="27" spans="1:12" ht="28">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12" t="s">
+    <row r="28" spans="1:12" ht="28">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C28" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31" t="s">
+      <c r="D28" s="12"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="13"/>
-      <c r="I27" s="17" t="s">
+      <c r="H28" s="13"/>
+      <c r="I28" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="J27" s="17" t="s">
+      <c r="J28" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="K27" s="17"/>
+      <c r="K28" s="17"/>
     </row>
-    <row r="28" spans="1:12" ht="28">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26" t="s">
+    <row r="29" spans="1:12" ht="28">
+      <c r="A29" s="26"/>
+      <c r="B29" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C29" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32" t="s">
+      <c r="D29" s="26"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="27"/>
-      <c r="I28" s="28" t="s">
+      <c r="H29" s="27"/>
+      <c r="I29" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="J28" s="28" t="s">
+      <c r="J29" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="K28" s="28"/>
+      <c r="K29" s="28"/>
     </row>
-    <row r="29" spans="1:12" ht="42">
-      <c r="A29" s="12" t="s">
+    <row r="30" spans="1:12" ht="42">
+      <c r="A30" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B30" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C30" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I29" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="K29" s="17"/>
-    </row>
-    <row r="30" spans="1:12" ht="70">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>41</v>
-      </c>
       <c r="D30" s="12"/>
-      <c r="E30" s="33"/>
+      <c r="E30" s="31"/>
       <c r="F30" s="31"/>
       <c r="G30" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="H30" s="17" t="s">
-        <v>67</v>
+      <c r="H30" s="12" t="s">
+        <v>66</v>
       </c>
-      <c r="I30" s="18" t="s">
-        <v>47</v>
+      <c r="I30" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="J30" s="17" t="s">
         <v>47</v>
       </c>
       <c r="K30" s="17"/>
     </row>
-    <row r="31" spans="1:12" ht="28">
-      <c r="A31" s="12" t="s">
-        <v>26</v>
+    <row r="31" spans="1:12" ht="70">
+      <c r="A31" s="12"/>
+      <c r="B31" s="13" t="s">
+        <v>40</v>
       </c>
-      <c r="B31" s="27" t="s">
-        <v>70</v>
+      <c r="C31" s="12" t="s">
+        <v>41</v>
       </c>
-      <c r="C31" s="27" t="s">
-        <v>74</v>
+      <c r="D31" s="12"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31" t="s">
+        <v>14</v>
       </c>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="28" t="s">
-        <v>68</v>
+      <c r="H31" s="17" t="s">
+        <v>67</v>
       </c>
-      <c r="I31" s="30" t="s">
+      <c r="I31" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="J31" s="28" t="s">
+      <c r="J31" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="K31" s="28"/>
+      <c r="K31" s="17"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" ht="28">
       <c r="A32" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D32" s="29"/>
       <c r="E32" s="29"/>
       <c r="F32" s="29"/>
       <c r="G32" s="29"/>
       <c r="H32" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I32" s="30" t="s">
         <v>47</v>
@@ -35709,31 +35708,47 @@
       </c>
       <c r="K32" s="28"/>
     </row>
-    <row r="33" spans="1:11" ht="28">
-      <c r="A33" s="26"/>
+    <row r="33" spans="1:11">
+      <c r="A33" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="B33" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
-      <c r="C33" s="27"/>
+      <c r="C33" s="27" t="s">
+        <v>72</v>
+      </c>
       <c r="D33" s="29"/>
       <c r="E33" s="29"/>
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
       <c r="H33" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="I33" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="J33" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="K33" s="28"/>
+    </row>
+    <row r="34" spans="1:11" ht="28">
+      <c r="A34" s="26"/>
+      <c r="B34" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="27"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="I33" s="23"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="10"/>
@@ -37571,7 +37586,7 @@
       <c r="F238" s="10"/>
       <c r="G238" s="10"/>
     </row>
-    <row r="239" spans="1:7" hidden="1">
+    <row r="239" spans="1:7">
       <c r="A239" s="10"/>
       <c r="B239" s="10"/>
       <c r="C239" s="10"/>
@@ -37697,7 +37712,7 @@
       <c r="F252" s="10"/>
       <c r="G252" s="10"/>
     </row>
-    <row r="253" spans="1:7">
+    <row r="253" spans="1:7" hidden="1">
       <c r="A253" s="10"/>
       <c r="B253" s="10"/>
       <c r="C253" s="10"/>
@@ -38579,13 +38594,22 @@
       <c r="F350" s="10"/>
       <c r="G350" s="10"/>
     </row>
+    <row r="351" spans="1:7">
+      <c r="A351" s="10"/>
+      <c r="B351" s="10"/>
+      <c r="C351" s="10"/>
+      <c r="D351" s="10"/>
+      <c r="E351" s="10"/>
+      <c r="F351" s="10"/>
+      <c r="G351" s="10"/>
+    </row>
   </sheetData>
   <sortState ref="A8:H35">
     <sortCondition ref="D8:D35"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A27:G27"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>